<commit_message>
Added pyproject.toml for deprecation, tested for numpy2. Seems no issues, so removed depency.
</commit_message>
<xml_diff>
--- a/docs/Examples/Other_features/Redox_Conversions.xlsx
+++ b/docs/Examples/Other_features/Redox_Conversions.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Other_features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Postdoc\MyBarometers\Thermobar_outer\docs\Examples\Other_features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351489B8-6A80-40F9-BEC2-F6CF113114EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F052AC-1972-4E63-9C31-0F4372B59964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{D90B9C4D-AEDD-428E-8035-F92B8F802A04}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{D90B9C4D-AEDD-428E-8035-F92B8F802A04}"/>
   </bookViews>
   <sheets>
     <sheet name="Liqs" sheetId="2" r:id="rId1"/>
     <sheet name="Pichavent_2018" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,12 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -251,7 +250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -357,7 +356,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,9 +520,9 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -571,7 +570,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -609,7 +608,7 @@
         <v>0.50827716249806898</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -647,7 +646,7 @@
         <v>0.51838589254652201</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -685,7 +684,7 @@
         <v>0.548285330219904</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -723,7 +722,7 @@
         <v>0.57126775420072595</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -761,7 +760,7 @@
         <v>0.61194021679709898</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -799,7 +798,7 @@
         <v>0.64056451096510303</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -837,7 +836,7 @@
         <v>0.68351945751144305</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -875,7 +874,7 @@
         <v>0.71218035450817097</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -913,7 +912,7 @@
         <v>0.75522824730414095</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -951,7 +950,7 @@
         <v>0.78397609572561799</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -989,7 +988,7 @@
         <v>0.82719119677003405</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>0.856074616430341</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>0.856074616430341</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>0.87054115223528805</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>0.885025476235627</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>0.89952850849714905</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1217,7 +1216,7 @@
         <v>0.91405116293225797</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>0.92991063713945599</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>0.97791205386944602</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1.02283973245167</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1369,7 +1368,7 @@
         <v>1.0629195665548099</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>1.10000930335469</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>1.1350808004977699</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>1.2324923240907699</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1521,7 +1520,7 @@
         <v>1.3566187488802699</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1559,7 +1558,7 @@
         <v>1.4411390432819799</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>1.5216923304905901</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>1.6240907626685199</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>1.6977529462244401</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>1.7691252602458101</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>1.8384905072420299</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>1.9282561756883401</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1825,7 +1824,7 @@
         <v>1.99379253230256</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>2.06041445911245</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>2.15284092249588</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>2.2206383836655599</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>2.2871265032876398</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2015,7 +2014,7 @@
         <v>2.3761678714891801</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>2.4412983441913698</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>2.5049827645681102</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>2.5876672850615501</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2167,7 +2166,7 @@
         <v>2.6480287671638001</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2205,7 +2204,7 @@
         <v>2.70699293858558</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>2.7645780626011902</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2281,7 +2280,7 @@
         <v>2.83924637288718</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>2.8936895901503501</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>2.94814747735508</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>3.0226627640291799</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2445,120 +2444,120 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2">
-        <v>72.599999999999994</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E2" s="2">
-        <v>14.7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.89</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="H2" s="2">
-        <v>3.99</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2.79</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1.85</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="C2">
+        <v>50.19</v>
+      </c>
+      <c r="D2">
+        <v>2.34</v>
+      </c>
+      <c r="E2">
+        <v>12.79</v>
+      </c>
+      <c r="F2">
+        <v>11.34</v>
+      </c>
+      <c r="G2">
+        <v>9.23</v>
+      </c>
+      <c r="H2">
+        <v>10.44</v>
+      </c>
+      <c r="I2">
+        <v>2.39</v>
+      </c>
+      <c r="J2">
+        <v>0.43</v>
+      </c>
+      <c r="K2">
         <v>92</v>
       </c>
-      <c r="L2" s="2">
-        <v>2.04</v>
-      </c>
-      <c r="M2" s="2">
-        <f>800+273.15</f>
-        <v>1073.1500000000001</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>1200+273.15</f>
+        <v>1473.15</v>
+      </c>
+      <c r="N2">
         <v>0.6</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>-13.8</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <f>10^O2</f>
         <v>1.5848931924611084E-14</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <f>P2*10</f>
         <v>1.5848931924611084E-13</v>
       </c>

</xml_diff>